<commit_message>
condicionales con archivo externo
</commit_message>
<xml_diff>
--- a/condicionales.xlsx
+++ b/condicionales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rstaffolani\Desktop\SALUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7296EF75-A785-43EE-A11A-89C91945C0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735C9594-B717-4C54-A767-D239611A475F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5F24D419-6351-49D0-9F46-CC25F658EA00}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E2784FDD-D670-4CC9-8FD3-538CDC5E4A22}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Regla</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Activa</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>aplicar_canalizador_localidad</t>
+  </si>
+  <si>
+    <t>aplicar_canalizador_provincia</t>
   </si>
 </sst>
 </file>
@@ -440,17 +449,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AE9CFB-63DE-4C02-AEAA-63EDD7CE8B56}">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746E806A-40AE-4DE5-99F6-87F739080711}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -469,12 +477,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -549,7 +557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -557,20 +565,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>